<commit_message>
- Tested all test setups to confirm that the system works fine before optimization
</commit_message>
<xml_diff>
--- a/src/output/opt/base/data.xlsx
+++ b/src/output/opt/base/data.xlsx
@@ -53,7 +53,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -62,15 +62,17 @@
     <col min="1" max="1" width="3.140625" customWidth="true"/>
     <col min="2" max="2" width="5.140625" customWidth="true"/>
     <col min="3" max="3" width="2.140625" customWidth="true"/>
-    <col min="4" max="4" width="2.140625" customWidth="true"/>
-    <col min="5" max="5" width="4.140625" customWidth="true"/>
-    <col min="6" max="6" width="4.7109375" customWidth="true"/>
-    <col min="7" max="7" width="4.140625" customWidth="true"/>
-    <col min="8" max="8" width="10.7109375" customWidth="true"/>
-    <col min="9" max="9" width="15.7109375" customWidth="true"/>
-    <col min="10" max="10" width="16.28515625" customWidth="true"/>
-    <col min="11" max="11" width="2.140625" customWidth="true"/>
-    <col min="12" max="12" width="3.140625" customWidth="true"/>
+    <col min="4" max="4" width="3.7109375" customWidth="true"/>
+    <col min="5" max="5" width="3.140625" customWidth="true"/>
+    <col min="6" max="6" width="4.140625" customWidth="true"/>
+    <col min="7" max="7" width="4.7109375" customWidth="true"/>
+    <col min="8" max="8" width="3.140625" customWidth="true"/>
+    <col min="9" max="9" width="4.140625" customWidth="true"/>
+    <col min="10" max="10" width="10.7109375" customWidth="true"/>
+    <col min="11" max="11" width="15.7109375" customWidth="true"/>
+    <col min="12" max="12" width="15.5703125" customWidth="true"/>
+    <col min="13" max="13" width="2.140625" customWidth="true"/>
+    <col min="14" max="14" width="3.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -84,30 +86,36 @@
         <v>5</v>
       </c>
       <c r="D1" s="0">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E1" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F1" s="0">
-        <v>0.94999999999999996</v>
+        <v>100</v>
       </c>
       <c r="G1" s="0">
-        <v>150</v>
+        <v>0.94999999999999996</v>
       </c>
       <c r="H1" s="0">
-        <v>30.5967348</v>
+        <v>10</v>
       </c>
       <c r="I1" s="0">
-        <v>0.00074060230656125547</v>
+        <v>209</v>
       </c>
       <c r="J1" s="0">
-        <v>5.9523013192408496e-06</v>
+        <v>11.7186302</v>
       </c>
       <c r="K1" s="0">
-        <v>0</v>
+        <v>6.3456254398186474e-05</v>
       </c>
       <c r="L1" s="0">
+        <v>7.0544782584561883e-07</v>
+      </c>
+      <c r="M1" s="0">
+        <v>0</v>
+      </c>
+      <c r="N1" s="0">
         <v>0</v>
       </c>
     </row>
@@ -122,30 +130,36 @@
         <v>5</v>
       </c>
       <c r="D2" s="0">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E2" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0">
-        <v>0.94999999999999996</v>
+        <v>100</v>
       </c>
       <c r="G2" s="0">
-        <v>153</v>
+        <v>0.94999999999999996</v>
       </c>
       <c r="H2" s="0">
-        <v>61.085683899999999</v>
+        <v>10</v>
       </c>
       <c r="I2" s="0">
-        <v>0.00074060230656125547</v>
+        <v>269</v>
       </c>
       <c r="J2" s="0">
-        <v>6.3049255174464555e-06</v>
+        <v>84.339021500000001</v>
       </c>
       <c r="K2" s="0">
-        <v>0</v>
+        <v>6.5997330021216882e-05</v>
       </c>
       <c r="L2" s="0">
+        <v>4.8492216979766602e-07</v>
+      </c>
+      <c r="M2" s="0">
+        <v>0</v>
+      </c>
+      <c r="N2" s="0">
         <v>0</v>
       </c>
     </row>
@@ -160,31 +174,37 @@
         <v>5</v>
       </c>
       <c r="D3" s="0">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E3" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0">
-        <v>0.94999999999999996</v>
+        <v>100</v>
       </c>
       <c r="G3" s="0">
-        <v>179</v>
+        <v>0.94999999999999996</v>
       </c>
       <c r="H3" s="0">
-        <v>74.751073399999996</v>
+        <v>10</v>
       </c>
       <c r="I3" s="0">
-        <v>0.00074060230656125547</v>
+        <v>251</v>
       </c>
       <c r="J3" s="0">
-        <v>-6.4932935239886316e-05</v>
+        <v>91.693737799999994</v>
       </c>
       <c r="K3" s="0">
+        <v>0.00020161746254965252</v>
+      </c>
+      <c r="L3" s="0">
+        <v>-2.3781491897126006e-05</v>
+      </c>
+      <c r="M3" s="0">
         <v>1</v>
       </c>
-      <c r="L3" s="0">
-        <v>27</v>
+      <c r="N3" s="0">
+        <v>83</v>
       </c>
     </row>
     <row r="4">
@@ -198,31 +218,37 @@
         <v>5</v>
       </c>
       <c r="D4" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E4" s="0">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0">
+        <v>100</v>
+      </c>
+      <c r="G4" s="0">
+        <v>0.94999999999999996</v>
+      </c>
+      <c r="H4" s="0">
+        <v>10</v>
+      </c>
+      <c r="I4" s="0">
+        <v>269</v>
+      </c>
+      <c r="J4" s="0">
+        <v>240.06703970000001</v>
+      </c>
+      <c r="K4" s="0">
+        <v>0.00078415626376182601</v>
+      </c>
+      <c r="L4" s="0">
+        <v>-3.0608607912803039e-05</v>
+      </c>
+      <c r="M4" s="0">
         <v>2</v>
       </c>
-      <c r="E4" s="0">
-        <v>100</v>
-      </c>
-      <c r="F4" s="0">
-        <v>0.94999999999999996</v>
-      </c>
-      <c r="G4" s="0">
-        <v>165</v>
-      </c>
-      <c r="H4" s="0">
-        <v>119.8789783</v>
-      </c>
-      <c r="I4" s="0">
-        <v>0.0014109080962998455</v>
-      </c>
-      <c r="J4" s="0">
-        <v>1.0492011084656754e-05</v>
-      </c>
-      <c r="K4" s="0">
-        <v>0</v>
-      </c>
-      <c r="L4" s="0">
-        <v>0</v>
+      <c r="N4" s="0">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>